<commit_message>
zaw - added login and book list doc
</commit_message>
<xml_diff>
--- a/documentation/03_詳細設計/画面設計/アカウント登録.xlsx
+++ b/documentation/03_詳細設計/画面設計/アカウント登録.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="7755" tabRatio="781"/>
+    <workbookView windowWidth="19815" windowHeight="7755" tabRatio="781" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="画面レイアウト" sheetId="20" r:id="rId1"/>
@@ -13,7 +13,6 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="G_APPLY_ID">#REF!</definedName>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="99">
   <si>
     <t>1．画面レイアウト</t>
   </si>
@@ -176,13 +175,13 @@
     <t>/book_list</t>
   </si>
   <si>
+    <t>POST</t>
+  </si>
+  <si>
     <t>/register</t>
   </si>
   <si>
     <t>/login</t>
-  </si>
-  <si>
-    <t>POST</t>
   </si>
   <si>
     <t>テーブル定義</t>
@@ -332,12 +331,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="46">
+  <fonts count="43">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,11 +402,6 @@
       <charset val="128"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="ＭＳ ゴシック"/>
-      <charset val="128"/>
-    </font>
-    <font>
       <b/>
       <i/>
       <u/>
@@ -482,21 +476,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="ＭＳ ゴシック"/>
@@ -525,6 +504,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -534,7 +527,114 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -547,129 +647,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="37">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -702,13 +681,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -720,19 +777,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -744,55 +801,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -810,79 +837,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1173,26 +1140,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1213,6 +1160,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1242,21 +1204,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1270,160 +1217,180 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="20" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="26" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="30" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="30" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="18" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="27" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="27" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1562,55 +1529,52 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
@@ -1619,46 +1583,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="16" xfId="42" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="16" xfId="42" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="17" xfId="42" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="17" xfId="42" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="18" xfId="42" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="17" xfId="42" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="17" xfId="42" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="18" xfId="42" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="19" xfId="42" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="19" xfId="42" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="19" xfId="42" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="19" xfId="42" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1">
@@ -1673,16 +1637,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
@@ -1694,22 +1658,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="0" xfId="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="17" xfId="42" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="17" xfId="42" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="21" xfId="42" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="42" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="19" xfId="42" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="19" xfId="42" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="22" xfId="42" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="22" xfId="42" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
@@ -1718,7 +1682,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
@@ -1807,7 +1771,7 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>90805</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[2]!make">
+    <xdr:sp macro="[1]!make">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="角丸四角形 1"/>
         <xdr:cNvSpPr/>
@@ -1956,26 +1920,6 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="テーブル定義"/>
-      <sheetName val="ワーク"/>
-      <sheetName val="user_ユーザーデータ"/>
-    </sheetNames>
-    <definedNames>
-      <definedName name="make"/>
-    </definedNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2284,8 +2228,8 @@
   <sheetPr/>
   <dimension ref="B1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2312,21 +2256,21 @@
       <c r="N2" s="28"/>
     </row>
     <row r="3" spans="2:15">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="91"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="90"/>
       <c r="O3" s="28"/>
     </row>
     <row r="4" spans="4:15">
@@ -2357,299 +2301,177 @@
       <c r="N5" s="28"/>
       <c r="O5" s="28"/>
     </row>
-    <row r="6" s="69" customFormat="1" spans="2:15">
-      <c r="B6" s="69" t="s">
+    <row r="6" s="68" customFormat="1" spans="2:15">
+      <c r="B6" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
-      <c r="N6" s="72"/>
-      <c r="O6" s="72"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="71"/>
+      <c r="L6" s="71"/>
+      <c r="M6" s="71"/>
+      <c r="N6" s="71"/>
+      <c r="O6" s="71"/>
     </row>
     <row r="8" spans="2:14">
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="74"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="74"/>
-      <c r="I8" s="92" t="s">
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="92"/>
-      <c r="K8" s="92" t="s">
+      <c r="J8" s="91"/>
+      <c r="K8" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="L8" s="92"/>
-      <c r="M8" s="92" t="s">
+      <c r="L8" s="91"/>
+      <c r="M8" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="N8" s="93"/>
+      <c r="N8" s="92"/>
     </row>
     <row r="9" spans="2:14">
-      <c r="B9" s="76"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="77"/>
-      <c r="I9" s="94"/>
-      <c r="J9" s="94"/>
-      <c r="K9" s="94"/>
-      <c r="L9" s="94"/>
-      <c r="M9" s="94"/>
-      <c r="N9" s="95"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="77"/>
+      <c r="G9" s="77"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="93"/>
+      <c r="J9" s="93"/>
+      <c r="K9" s="93"/>
+      <c r="L9" s="93"/>
+      <c r="M9" s="93"/>
+      <c r="N9" s="94"/>
     </row>
     <row r="10" spans="2:14">
-      <c r="B10" s="79"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="80"/>
-      <c r="H10" s="80"/>
-      <c r="I10" s="80"/>
-      <c r="J10" s="80"/>
-      <c r="K10" s="80"/>
-      <c r="L10" s="80"/>
-      <c r="M10" s="80"/>
-      <c r="N10" s="96"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="79"/>
+      <c r="I10" s="79"/>
+      <c r="J10" s="79"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="79"/>
+      <c r="M10" s="79"/>
+      <c r="N10" s="95"/>
     </row>
     <row r="11" spans="2:14">
-      <c r="B11" s="81"/>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11" s="82" t="s">
+      <c r="B11" s="80"/>
+      <c r="F11" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="82"/>
-      <c r="H11" s="82"/>
-      <c r="I11" s="82"/>
-      <c r="J11"/>
-      <c r="K11"/>
-      <c r="L11"/>
-      <c r="M11"/>
-      <c r="N11" s="97"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="N11" s="96"/>
     </row>
     <row r="12" spans="2:14">
-      <c r="B12" s="81"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12" s="82"/>
-      <c r="G12" s="82"/>
-      <c r="H12" s="82"/>
-      <c r="I12" s="82"/>
-      <c r="J12"/>
-      <c r="K12"/>
-      <c r="L12"/>
-      <c r="M12"/>
-      <c r="N12" s="97"/>
+      <c r="B12" s="80"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
+      <c r="N12" s="96"/>
     </row>
     <row r="13" spans="2:14">
-      <c r="B13" s="81"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13"/>
-      <c r="J13"/>
-      <c r="K13"/>
-      <c r="L13"/>
-      <c r="M13"/>
-      <c r="N13" s="97"/>
+      <c r="B13" s="80"/>
+      <c r="N13" s="96"/>
     </row>
     <row r="14" spans="2:14">
-      <c r="B14" s="81"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14"/>
-      <c r="J14"/>
-      <c r="K14"/>
-      <c r="L14"/>
-      <c r="M14"/>
-      <c r="N14" s="97"/>
+      <c r="B14" s="80"/>
+      <c r="N14" s="96"/>
     </row>
     <row r="15" spans="2:14">
-      <c r="B15" s="81"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
+      <c r="B15" s="80"/>
       <c r="F15" t="s">
         <v>8</v>
       </c>
-      <c r="G15"/>
-      <c r="H15"/>
-      <c r="I15"/>
-      <c r="J15"/>
-      <c r="K15"/>
-      <c r="L15"/>
-      <c r="M15"/>
-      <c r="N15" s="97"/>
+      <c r="N15" s="96"/>
     </row>
     <row r="16" spans="2:14">
-      <c r="B16" s="81"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16" s="83" t="s">
+      <c r="B16" s="80"/>
+      <c r="F16" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="84"/>
-      <c r="H16" s="84"/>
-      <c r="I16" s="98"/>
-      <c r="J16"/>
-      <c r="K16"/>
-      <c r="L16"/>
-      <c r="M16"/>
-      <c r="N16" s="97"/>
+      <c r="G16" s="83"/>
+      <c r="H16" s="83"/>
+      <c r="I16" s="97"/>
+      <c r="N16" s="96"/>
     </row>
     <row r="17" spans="2:14">
-      <c r="B17" s="81"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17"/>
-      <c r="G17"/>
-      <c r="H17"/>
-      <c r="I17"/>
-      <c r="J17"/>
-      <c r="K17"/>
-      <c r="L17"/>
-      <c r="M17"/>
-      <c r="N17" s="97"/>
+      <c r="B17" s="80"/>
+      <c r="N17" s="96"/>
     </row>
     <row r="18" spans="2:14">
-      <c r="B18" s="81"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
+      <c r="B18" s="80"/>
       <c r="F18" t="s">
         <v>10</v>
       </c>
-      <c r="G18"/>
-      <c r="H18"/>
-      <c r="I18"/>
-      <c r="J18"/>
-      <c r="K18"/>
-      <c r="L18"/>
-      <c r="M18"/>
-      <c r="N18" s="97"/>
+      <c r="N18" s="96"/>
     </row>
     <row r="19" spans="2:14">
-      <c r="B19" s="81"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19" s="83" t="s">
+      <c r="B19" s="80"/>
+      <c r="F19" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="84"/>
-      <c r="H19" s="84"/>
-      <c r="I19" s="98"/>
-      <c r="J19"/>
-      <c r="K19"/>
-      <c r="L19"/>
-      <c r="M19"/>
-      <c r="N19" s="97"/>
+      <c r="G19" s="83"/>
+      <c r="H19" s="83"/>
+      <c r="I19" s="97"/>
+      <c r="N19" s="96"/>
     </row>
     <row r="20" spans="2:14">
-      <c r="B20" s="81"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20"/>
-      <c r="J20"/>
-      <c r="K20"/>
-      <c r="L20"/>
-      <c r="M20"/>
-      <c r="N20" s="97"/>
+      <c r="B20" s="80"/>
+      <c r="N20" s="96"/>
     </row>
     <row r="21" spans="2:14">
-      <c r="B21" s="81"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21" s="85" t="s">
+      <c r="B21" s="80"/>
+      <c r="F21" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="86"/>
-      <c r="H21"/>
-      <c r="I21"/>
-      <c r="J21"/>
-      <c r="K21"/>
-      <c r="L21"/>
-      <c r="M21"/>
-      <c r="N21" s="97"/>
+      <c r="G21" s="85"/>
+      <c r="N21" s="96"/>
     </row>
     <row r="22" spans="2:14">
-      <c r="B22" s="81"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22" s="87"/>
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
-      <c r="J22"/>
-      <c r="K22"/>
-      <c r="L22"/>
-      <c r="M22"/>
-      <c r="N22" s="97"/>
+      <c r="B22" s="80"/>
+      <c r="F22" s="86"/>
+      <c r="N22" s="96"/>
     </row>
     <row r="23" spans="2:14">
-      <c r="B23" s="81"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23"/>
-      <c r="I23"/>
-      <c r="J23"/>
-      <c r="K23"/>
-      <c r="L23"/>
-      <c r="M23"/>
-      <c r="N23" s="97"/>
+      <c r="B23" s="80"/>
+      <c r="N23" s="96"/>
     </row>
     <row r="24" spans="2:14">
-      <c r="B24" s="88"/>
-      <c r="C24" s="89"/>
-      <c r="D24" s="89"/>
-      <c r="E24" s="89"/>
-      <c r="F24" s="89"/>
-      <c r="G24" s="89"/>
-      <c r="H24" s="89"/>
-      <c r="I24" s="89"/>
-      <c r="J24" s="89"/>
-      <c r="K24" s="89"/>
-      <c r="L24" s="89"/>
-      <c r="M24" s="89"/>
-      <c r="N24" s="99"/>
+      <c r="B24" s="87"/>
+      <c r="C24" s="88"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="88"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="88"/>
+      <c r="I24" s="88"/>
+      <c r="J24" s="88"/>
+      <c r="K24" s="88"/>
+      <c r="L24" s="88"/>
+      <c r="M24" s="88"/>
+      <c r="N24" s="98"/>
     </row>
     <row r="30" spans="2:2">
-      <c r="B30" s="69"/>
+      <c r="B30" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2671,10 +2493,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B1:P88"/>
+  <dimension ref="B1:P87"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2719,8 +2541,8 @@
       <c r="I3" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="62"/>
     </row>
     <row r="4" spans="2:11">
       <c r="B4" s="33">
@@ -2743,8 +2565,8 @@
       </c>
       <c r="H4" s="33"/>
       <c r="I4" s="44"/>
-      <c r="J4" s="63"/>
-      <c r="K4" s="63"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
     </row>
     <row r="5" spans="2:11">
       <c r="B5" s="33">
@@ -2767,8 +2589,8 @@
       </c>
       <c r="H5" s="33"/>
       <c r="I5" s="44"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
     </row>
     <row r="6" spans="2:11">
       <c r="B6" s="33">
@@ -2791,8 +2613,8 @@
       </c>
       <c r="H6" s="33"/>
       <c r="I6" s="44"/>
-      <c r="J6" s="63"/>
-      <c r="K6" s="63"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
     </row>
     <row r="7" spans="2:11">
       <c r="B7" s="33">
@@ -2815,8 +2637,8 @@
       </c>
       <c r="H7" s="33"/>
       <c r="I7" s="44"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="63"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
     </row>
     <row r="8" spans="2:11">
       <c r="B8" s="33">
@@ -2838,9 +2660,9 @@
         <v>26</v>
       </c>
       <c r="H8" s="38"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="63"/>
-      <c r="K8" s="63"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
     </row>
     <row r="9" spans="2:11">
       <c r="B9" s="33">
@@ -2867,8 +2689,8 @@
       <c r="I9" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="J9" s="63"/>
-      <c r="K9" s="63"/>
+      <c r="J9" s="62"/>
+      <c r="K9" s="62"/>
     </row>
     <row r="10" spans="2:11">
       <c r="B10" s="33">
@@ -2891,8 +2713,8 @@
       </c>
       <c r="H10" s="45"/>
       <c r="I10" s="44"/>
-      <c r="J10" s="63"/>
-      <c r="K10" s="63"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="62"/>
     </row>
     <row r="11" spans="2:11">
       <c r="B11" s="33">
@@ -2915,8 +2737,8 @@
       </c>
       <c r="H11" s="45"/>
       <c r="I11" s="44"/>
-      <c r="J11" s="63"/>
-      <c r="K11" s="63"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="62"/>
     </row>
     <row r="12" spans="2:11">
       <c r="B12" s="33">
@@ -2943,8 +2765,8 @@
       <c r="I12" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="J12" s="63"/>
-      <c r="K12" s="63"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="62"/>
     </row>
     <row r="13" spans="2:11">
       <c r="B13" s="33">
@@ -2969,8 +2791,8 @@
       <c r="I13" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="J13" s="63"/>
-      <c r="K13" s="63"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
     </row>
     <row r="14" spans="11:11">
       <c r="K14" s="28"/>
@@ -3017,7 +2839,7 @@
       </c>
       <c r="G18" s="54"/>
       <c r="H18" s="55"/>
-      <c r="I18" s="65" t="s">
+      <c r="I18" s="64" t="s">
         <v>21</v>
       </c>
       <c r="K18" s="28"/>
@@ -3040,14 +2862,14 @@
       </c>
       <c r="G19" s="59"/>
       <c r="H19" s="60"/>
-      <c r="I19" s="62"/>
+      <c r="I19" s="61"/>
       <c r="K19" s="28"/>
     </row>
     <row r="20" customFormat="1" spans="2:10">
       <c r="B20" s="56">
         <v>2</v>
       </c>
-      <c r="C20" s="61" t="s">
+      <c r="C20" s="36" t="s">
         <v>23</v>
       </c>
       <c r="D20" s="57" t="s">
@@ -3061,14 +2883,14 @@
       </c>
       <c r="G20" s="59"/>
       <c r="H20" s="60"/>
-      <c r="I20" s="66"/>
+      <c r="I20" s="65"/>
       <c r="J20" s="28"/>
     </row>
     <row r="21" customFormat="1" spans="2:10">
       <c r="B21" s="56">
         <v>3</v>
       </c>
-      <c r="C21" s="61" t="s">
+      <c r="C21" s="36" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="57" t="s">
@@ -3082,7 +2904,7 @@
       </c>
       <c r="G21" s="59"/>
       <c r="H21" s="60"/>
-      <c r="I21" s="67"/>
+      <c r="I21" s="66"/>
       <c r="J21" s="28"/>
     </row>
     <row r="22" s="27" customFormat="1" spans="2:10">
@@ -3095,16 +2917,16 @@
       <c r="D22" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="57" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" s="62" t="s">
+      <c r="E22" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="G22" s="62"/>
-      <c r="H22" s="62"/>
-      <c r="I22" s="66"/>
-      <c r="J22" s="63"/>
+      <c r="F22" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="65"/>
+      <c r="J22" s="62"/>
     </row>
     <row r="23" s="27" customFormat="1" spans="2:10">
       <c r="B23" s="56">
@@ -3119,13 +2941,13 @@
       <c r="E23" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="62" t="s">
-        <v>50</v>
-      </c>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="66"/>
-      <c r="J23" s="63"/>
+      <c r="F23" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="65"/>
+      <c r="J23" s="62"/>
     </row>
     <row r="24" ht="14" customHeight="1" spans="2:9">
       <c r="B24" s="56">
@@ -3138,53 +2960,36 @@
         <v>39</v>
       </c>
       <c r="E24" s="56" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F24" s="58" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G24" s="59"/>
       <c r="H24" s="60"/>
-      <c r="I24" s="68"/>
-    </row>
-    <row r="25" ht="14" customHeight="1" spans="2:9">
-      <c r="B25" s="56">
-        <v>7</v>
-      </c>
-      <c r="C25" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="F25" s="58" t="s">
-        <v>50</v>
-      </c>
+      <c r="I24" s="67"/>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="58"/>
       <c r="G25" s="59"/>
       <c r="H25" s="60"/>
-      <c r="I25" s="44"/>
-    </row>
-    <row r="26" spans="2:9">
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="59"/>
-      <c r="H26" s="60"/>
-      <c r="I26" s="41"/>
+      <c r="I25" s="41"/>
+    </row>
+    <row r="33" s="27" customFormat="1" spans="10:10">
+      <c r="J33" s="62"/>
     </row>
     <row r="34" s="27" customFormat="1" spans="10:10">
-      <c r="J34" s="63"/>
+      <c r="J34" s="62"/>
     </row>
     <row r="35" s="27" customFormat="1" spans="10:10">
-      <c r="J35" s="63"/>
-    </row>
-    <row r="36" s="27" customFormat="1" spans="10:10">
-      <c r="J36" s="63"/>
+      <c r="J35" s="62"/>
+    </row>
+    <row r="39" spans="11:11">
+      <c r="K39" s="28"/>
     </row>
     <row r="40" spans="11:11">
       <c r="K40" s="28"/>
@@ -3201,35 +3006,36 @@
     <row r="44" spans="11:11">
       <c r="K44" s="28"/>
     </row>
-    <row r="45" spans="11:11">
-      <c r="K45" s="28"/>
+    <row r="60" s="27" customFormat="1" spans="10:10">
+      <c r="J60" s="62"/>
     </row>
     <row r="61" s="27" customFormat="1" spans="10:10">
-      <c r="J61" s="63"/>
-    </row>
-    <row r="62" s="27" customFormat="1" spans="10:10">
-      <c r="J62" s="63"/>
+      <c r="J61" s="62"/>
+    </row>
+    <row r="71" spans="10:10">
+      <c r="J71"/>
     </row>
     <row r="72" spans="10:10">
       <c r="J72"/>
     </row>
-    <row r="73" spans="10:10">
-      <c r="J73"/>
+    <row r="78" s="27" customFormat="1" spans="10:10">
+      <c r="J78" s="62"/>
     </row>
     <row r="79" s="27" customFormat="1" spans="10:10">
-      <c r="J79" s="63"/>
+      <c r="J79" s="62"/>
     </row>
     <row r="80" s="27" customFormat="1" spans="10:10">
-      <c r="J80" s="63"/>
+      <c r="J80" s="62"/>
     </row>
     <row r="81" s="27" customFormat="1" spans="10:10">
-      <c r="J81" s="63"/>
+      <c r="J81" s="62"/>
     </row>
     <row r="82" s="27" customFormat="1" spans="10:10">
-      <c r="J82" s="63"/>
-    </row>
-    <row r="83" s="27" customFormat="1" spans="10:10">
-      <c r="J83" s="63"/>
+      <c r="J82" s="62"/>
+    </row>
+    <row r="83" spans="15:16">
+      <c r="O83" s="27"/>
+      <c r="P83" s="27"/>
     </row>
     <row r="84" spans="15:16">
       <c r="O84" s="27"/>
@@ -3247,12 +3053,8 @@
       <c r="O87" s="27"/>
       <c r="P87" s="27"/>
     </row>
-    <row r="88" spans="15:16">
-      <c r="O88" s="27"/>
-      <c r="P88" s="27"/>
-    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="8">
     <mergeCell ref="F18:H18"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="F20:H20"/>
@@ -3261,7 +3063,6 @@
     <mergeCell ref="F23:H23"/>
     <mergeCell ref="F24:H24"/>
     <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F26:H26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3765,7 +3566,7 @@
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 F9 F10 F5:F8 F11:F12 F13:F14 F15:F16">
-      <formula1>[2]データ!#REF!</formula1>
+      <formula1>[1]データ!#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
       <formula1>"○,　"</formula1>

</xml_diff>